<commit_message>
Dynamic Token Models to be obtain via plist
Tokens moved to a circular shape for easier shape mapping.

Signed-off-by: Chris <cdesch@gmail.com>
</commit_message>
<xml_diff>
--- a/AppImages/GameObjects/CoinScales.xlsx
+++ b/AppImages/GameObjects/CoinScales.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="12760" yWindow="4400" windowWidth="25500" windowHeight="10200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -49,6 +49,22 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,14 +84,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,10 +441,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F6"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A3:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -470,7 +507,7 @@
         <v>0.73821989528795806</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:E6" si="0">D4*C5</f>
+        <f t="shared" ref="D5:D6" si="0">D4*C5</f>
         <v>20.654696965543707</v>
       </c>
       <c r="E5">
@@ -506,8 +543,65 @@
         <v>100.52356020942409</v>
       </c>
     </row>
+    <row r="8" spans="1:6">
+      <c r="D8">
+        <f>D3/2</f>
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:F8" si="1">E3/2</f>
+        <v>32</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="D9">
+        <f t="shared" ref="D9:F11" si="2">D4/2</f>
+        <v>13.989528795811518</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>27.979057591623036</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>55.958115183246072</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>10.327348482771853</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>23.623036649214658</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>47.246073298429316</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>8.1104831016532888</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>25.130890052356023</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>50.261780104712045</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="F5" formula="1"/>
   </ignoredErrors>

</xml_diff>